<commit_message>
[docs] [fix] [shell] [flutter] [新增 flutter 相關說明文件]
# [docs] [fix] [shell] [flutter] [新增 flutter 相關說明文件]

更新資料，有部分有遺漏
</commit_message>
<xml_diff>
--- a/doc/shell/flutter/backup/技術研究.xlsx
+++ b/doc/shell/flutter/backup/技術研究.xlsx
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="183">
   <si>
     <t>項目</t>
   </si>
@@ -990,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1111,9 +1111,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -13351,7 +13348,9 @@
       <c r="D48" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="43"/>
+      <c r="E48" s="42" t="s">
+        <v>45</v>
+      </c>
       <c r="F48" s="2" t="s">
         <v>45</v>
       </c>
@@ -13565,16 +13564,16 @@
       <c r="AB56" s="27"/>
     </row>
     <row r="57" hidden="1">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="43" t="s">
         <v>78</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C57" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="45" t="s">
+      <c r="C57" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="44" t="s">
         <v>46</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -13592,7 +13591,7 @@
       <c r="I57" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="46" t="s">
+      <c r="J57" s="45" t="s">
         <v>79</v>
       </c>
     </row>
@@ -13661,22 +13660,22 @@
       </c>
     </row>
     <row r="60" hidden="1">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="43" t="s">
         <v>84</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C60" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60" s="45" t="s">
+      <c r="C60" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="44" t="s">
         <v>46</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F60" s="44" t="s">
         <v>46</v>
       </c>
       <c r="G60" s="2" t="s">
@@ -13688,7 +13687,7 @@
       <c r="I60" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J60" s="46" t="s">
+      <c r="J60" s="45" t="s">
         <v>85</v>
       </c>
     </row>
@@ -14111,7 +14110,7 @@
       <c r="AB78" s="37"/>
     </row>
     <row r="79">
-      <c r="A79" s="47" t="s">
+      <c r="A79" s="46" t="s">
         <v>160</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -14138,12 +14137,12 @@
       <c r="I79" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J79" s="48" t="s">
+      <c r="J79" s="47" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="46" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -14170,7 +14169,7 @@
       <c r="I80" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J80" s="48" t="s">
+      <c r="J80" s="47" t="s">
         <v>163</v>
       </c>
     </row>
@@ -14219,7 +14218,7 @@
       <c r="AB82" s="37"/>
     </row>
     <row r="83" hidden="1">
-      <c r="A83" s="44" t="s">
+      <c r="A83" s="43" t="s">
         <v>99</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -14231,7 +14230,7 @@
       <c r="D83" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E83" s="45" t="s">
+      <c r="E83" s="44" t="s">
         <v>46</v>
       </c>
       <c r="F83" s="2" t="s">
@@ -14246,12 +14245,12 @@
       <c r="I83" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J83" s="46" t="s">
+      <c r="J83" s="45" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="84" hidden="1">
-      <c r="A84" s="44" t="s">
+      <c r="A84" s="43" t="s">
         <v>101</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -14263,7 +14262,7 @@
       <c r="D84" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E84" s="45" t="s">
+      <c r="E84" s="44" t="s">
         <v>46</v>
       </c>
       <c r="F84" s="2" t="s">
@@ -14278,12 +14277,12 @@
       <c r="I84" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J84" s="46" t="s">
+      <c r="J84" s="45" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="85" hidden="1">
-      <c r="A85" s="44" t="s">
+      <c r="A85" s="43" t="s">
         <v>103</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -14295,7 +14294,7 @@
       <c r="D85" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E85" s="45" t="s">
+      <c r="E85" s="44" t="s">
         <v>46</v>
       </c>
       <c r="F85" s="2" t="s">
@@ -14310,7 +14309,7 @@
       <c r="I85" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J85" s="46" t="s">
+      <c r="J85" s="45" t="s">
         <v>104</v>
       </c>
     </row>
@@ -14342,7 +14341,7 @@
       <c r="I86" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J86" s="49" t="s">
+      <c r="J86" s="48" t="s">
         <v>164</v>
       </c>
     </row>
@@ -14374,12 +14373,12 @@
       <c r="I87" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J87" s="49" t="s">
+      <c r="J87" s="48" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="88" hidden="1">
-      <c r="A88" s="44" t="s">
+      <c r="A88" s="43" t="s">
         <v>109</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -14391,7 +14390,7 @@
       <c r="D88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E88" s="45" t="s">
+      <c r="E88" s="44" t="s">
         <v>46</v>
       </c>
       <c r="F88" s="2" t="s">
@@ -14406,7 +14405,7 @@
       <c r="I88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J88" s="46" t="s">
+      <c r="J88" s="45" t="s">
         <v>110</v>
       </c>
     </row>
@@ -14482,7 +14481,7 @@
       <c r="I91" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J91" s="49" t="s">
+      <c r="J91" s="48" t="s">
         <v>166</v>
       </c>
     </row>
@@ -14514,7 +14513,7 @@
       <c r="I92" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J92" s="49" t="s">
+      <c r="J92" s="48" t="s">
         <v>167</v>
       </c>
     </row>
@@ -14546,7 +14545,7 @@
       <c r="I93" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J93" s="49" t="s">
+      <c r="J93" s="48" t="s">
         <v>168</v>
       </c>
     </row>
@@ -14595,7 +14594,7 @@
       <c r="AB95" s="37"/>
     </row>
     <row r="96" hidden="1">
-      <c r="A96" s="44" t="s">
+      <c r="A96" s="43" t="s">
         <v>117</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -14622,12 +14621,12 @@
       <c r="I96" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J96" s="46" t="s">
+      <c r="J96" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="97" hidden="1">
-      <c r="A97" s="44" t="s">
+      <c r="A97" s="43" t="s">
         <v>119</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -14654,7 +14653,7 @@
       <c r="I97" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J97" s="46" t="s">
+      <c r="J97" s="45" t="s">
         <v>120</v>
       </c>
     </row>
@@ -14686,7 +14685,7 @@
       <c r="I98" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J98" s="49" t="s">
+      <c r="J98" s="48" t="s">
         <v>169</v>
       </c>
     </row>
@@ -14718,7 +14717,7 @@
       <c r="I99" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J99" s="49" t="s">
+      <c r="J99" s="48" t="s">
         <v>170</v>
       </c>
     </row>
@@ -25720,62 +25719,62 @@
   </cols>
   <sheetData>
     <row r="9">
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10">
-      <c r="C10" s="51"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11">
-      <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
     </row>
     <row r="12">
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="51"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13">
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="15">
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16">
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17">
-      <c r="C17" s="51"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18">
-      <c r="C18" s="51"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="51"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19">
-      <c r="C19" s="51"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>